<commit_message>
Updating the economic indexer data
Updating the economic indexer data
</commit_message>
<xml_diff>
--- a/indexer_lib/data/CDI mensal.xlsx
+++ b/indexer_lib/data/CDI mensal.xlsx
@@ -479,6 +479,15 @@
       <c r="E2" s="2">
         <v>0.20780000000000001</v>
       </c>
+      <c r="F2" s="2">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.30780000000000002</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.35560000000000003</v>
+      </c>
       <c r="O2" t="s">
         <v>14</v>
       </c>

</xml_diff>